<commit_message>
completed test for CPQ Booking; updated BE tests
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18792" windowHeight="9487" activeTab="3"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="127">
   <si>
     <t>Tag</t>
   </si>
@@ -226,6 +226,18 @@
     <t>3M#$,qns5uw*W#jr</t>
   </si>
   <si>
+    <t>SALESFORCECPQUSER</t>
+  </si>
+  <si>
+    <t>oksanasysadmincpq@bpp.com.noahqa</t>
+  </si>
+  <si>
+    <t>SALESFORCECPQPASSWORD</t>
+  </si>
+  <si>
+    <t>12space34</t>
+  </si>
+  <si>
     <t>ENTER</t>
   </si>
   <si>
@@ -365,6 +377,12 @@
   </si>
   <si>
     <t>http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/</t>
+  </si>
+  <si>
+    <t>SALESFORCEINSTANCE</t>
+  </si>
+  <si>
+    <t>https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -387,10 +405,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -447,14 +465,128 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,120 +599,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -591,187 +609,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,12 +816,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -827,47 +858,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,158 +882,184 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1050,9 +1068,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1070,6 +1085,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1393,18 +1414,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6605504587156" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1651376146789" style="11" customWidth="1"/>
-    <col min="2" max="2" width="45.5045871559633" style="11" customWidth="1"/>
-    <col min="3" max="3" width="44.1651376146789" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="8.6605504587156" style="11"/>
+    <col min="1" max="1" width="38.1651376146789" style="10" customWidth="1"/>
+    <col min="2" max="2" width="45.5045871559633" style="10" customWidth="1"/>
+    <col min="3" max="3" width="44.1651376146789" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="8.6605504587156" style="10"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1419,376 +1440,398 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" s="8" customFormat="1" spans="1:3">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" s="7" customFormat="1" spans="1:3">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" s="8" customFormat="1" spans="1:3">
-      <c r="A13" s="8" t="s">
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" s="7" customFormat="1" spans="1:3">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" s="8" customFormat="1" spans="1:3">
-      <c r="A14" s="8" t="s">
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" s="7" customFormat="1" spans="1:3">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" s="8" customFormat="1" spans="1:3">
-      <c r="A15" s="8" t="s">
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" s="7" customFormat="1" spans="1:3">
+      <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" s="8" customFormat="1" spans="1:3">
-      <c r="A16" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" s="7" customFormat="1" spans="1:3">
+      <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" s="8" customFormat="1" spans="1:3">
-      <c r="A17" s="8" t="s">
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" s="7" customFormat="1" spans="1:3">
+      <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" s="8" customFormat="1" spans="1:3">
-      <c r="A18" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" s="7" customFormat="1" spans="1:3">
+      <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" s="8" customFormat="1" spans="1:3">
-      <c r="A19" s="8" t="s">
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" s="7" customFormat="1" spans="1:3">
+      <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" s="8" customFormat="1" spans="1:3">
-      <c r="A20" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" s="7" customFormat="1" spans="1:3">
+      <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" s="8" customFormat="1" spans="1:3">
-      <c r="A21" s="8" t="s">
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" s="7" customFormat="1" spans="1:3">
+      <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" s="8" customFormat="1" spans="1:3">
-      <c r="A32" s="8" t="s">
+      <c r="C31" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" s="7" customFormat="1" spans="1:3">
+      <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" s="8" customFormat="1" spans="1:3">
-      <c r="A33" s="8" t="s">
+      <c r="C32" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" s="7" customFormat="1" spans="1:3">
+      <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1799,6 +1842,7 @@
     <hyperlink ref="B20" r:id="rId1" display="neo4j"/>
     <hyperlink ref="B22" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
     <hyperlink ref="B32" r:id="rId4" display="nadineanja@yahoo.com"/>
+    <hyperlink ref="B36" r:id="rId5" display="oksanasysadmincpq@bpp.com.noahqa"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1835,10 +1879,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1846,10 +1890,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1857,10 +1901,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1868,10 +1912,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1879,10 +1923,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1890,10 +1934,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1901,10 +1945,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1920,16 +1964,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.6605504587156" customWidth="1"/>
+    <col min="2" max="2" width="58.2752293577982" customWidth="1"/>
     <col min="3" max="3" width="26.1651376146789" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1946,10 +1990,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1957,10 +2001,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1968,10 +2012,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1979,10 +2023,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1990,10 +2034,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2001,10 +2045,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2012,10 +2056,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2023,10 +2067,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2034,98 +2078,98 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" s="5" customFormat="1" spans="1:3">
-      <c r="A11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="8" t="s">
+    <row r="11" s="4" customFormat="1" spans="1:3">
+      <c r="A11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -2133,23 +2177,34 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2165,6 +2220,7 @@
     <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
     <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
     <hyperlink ref="B20" r:id="rId9" display="http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/"/>
+    <hyperlink ref="B21" r:id="rId10" display="https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2177,7 +2233,7 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2201,10 +2257,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2212,23 +2268,23 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="2">
         <v>2381626</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated CPQ test foe UAT (including Metadata files) added new Locators for Hub
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
   <si>
     <t>Tag</t>
   </si>
@@ -398,6 +398,18 @@
   </si>
   <si>
     <t>SFOFFERING</t>
+  </si>
+  <si>
+    <t>SFCPQPRODUCT</t>
+  </si>
+  <si>
+    <t>SF CPQ test - SF CPQ test - SF CPQ flow test - London - Classroom - AutoTest Sitting</t>
+  </si>
+  <si>
+    <t>SFCPQINSTANCENUMBER</t>
+  </si>
+  <si>
+    <t>I-1443</t>
   </si>
 </sst>
 </file>
@@ -465,14 +477,128 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,120 +611,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -609,25 +621,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,157 +801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,21 +828,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -851,15 +848,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -888,6 +876,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -905,18 +904,31 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -934,128 +946,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1068,6 +1080,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1085,12 +1103,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1422,10 +1434,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6605504587156" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1651376146789" style="10" customWidth="1"/>
-    <col min="2" max="2" width="45.5045871559633" style="10" customWidth="1"/>
-    <col min="3" max="3" width="44.1651376146789" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="8.6605504587156" style="10"/>
+    <col min="1" max="1" width="38.1651376146789" style="12" customWidth="1"/>
+    <col min="2" max="2" width="45.5045871559633" style="12" customWidth="1"/>
+    <col min="3" max="3" width="44.1651376146789" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="8.6605504587156" style="12"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1440,398 +1452,398 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" s="7" customFormat="1" spans="1:3">
-      <c r="A12" s="7" t="s">
+      <c r="C11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" s="9" customFormat="1" spans="1:3">
+      <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" s="7" customFormat="1" spans="1:3">
-      <c r="A13" s="7" t="s">
+      <c r="C12" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" s="9" customFormat="1" spans="1:3">
+      <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" s="7" customFormat="1" spans="1:3">
-      <c r="A14" s="7" t="s">
+      <c r="C13" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" s="9" customFormat="1" spans="1:3">
+      <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" s="7" customFormat="1" spans="1:3">
-      <c r="A15" s="7" t="s">
+      <c r="C14" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" s="9" customFormat="1" spans="1:3">
+      <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
-      <c r="A16" s="7" t="s">
+      <c r="C15" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" s="9" customFormat="1" spans="1:3">
+      <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
-      <c r="A17" s="7" t="s">
+      <c r="C16" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" s="9" customFormat="1" spans="1:3">
+      <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" s="7" customFormat="1" spans="1:3">
-      <c r="A18" s="7" t="s">
+      <c r="C17" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" s="9" customFormat="1" spans="1:3">
+      <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" s="7" customFormat="1" spans="1:3">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" s="9" customFormat="1" spans="1:3">
+      <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" s="7" customFormat="1" spans="1:3">
-      <c r="A20" s="7" t="s">
+      <c r="C19" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" s="9" customFormat="1" spans="1:3">
+      <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" s="7" customFormat="1" spans="1:3">
-      <c r="A21" s="7" t="s">
+      <c r="C20" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" s="9" customFormat="1" spans="1:3">
+      <c r="A21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" s="7" customFormat="1" spans="1:3">
-      <c r="A32" s="7" t="s">
+      <c r="C31" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" s="9" customFormat="1" spans="1:3">
+      <c r="A32" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" s="7" customFormat="1" spans="1:3">
-      <c r="A33" s="7" t="s">
+      <c r="C32" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" s="9" customFormat="1" spans="1:3">
+      <c r="A33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1966,7 +1978,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1992,7 +2004,7 @@
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2003,7 +2015,7 @@
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2014,7 +2026,7 @@
       <c r="A4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2025,7 +2037,7 @@
       <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2036,7 +2048,7 @@
       <c r="A6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2047,7 +2059,7 @@
       <c r="A7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2058,7 +2070,7 @@
       <c r="A8" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2069,7 +2081,7 @@
       <c r="A9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2080,21 +2092,21 @@
       <c r="A10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:3">
-      <c r="A11" s="7" t="s">
+    <row r="11" s="6" customFormat="1" spans="1:3">
+      <c r="A11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2102,10 +2114,10 @@
       <c r="A12" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2113,10 +2125,10 @@
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2124,10 +2136,10 @@
       <c r="A14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2143,24 +2155,24 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2179,10 +2191,10 @@
       <c r="A19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2190,21 +2202,21 @@
       <c r="A20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2231,13 +2243,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="26.6605504587156" customWidth="1"/>
     <col min="2" max="2" width="34.5045871559633" customWidth="1"/>
@@ -2288,6 +2300,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
updated test for CPQ user
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="133">
   <si>
     <t>Tag</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>I-1443</t>
+  </si>
+  <si>
+    <t>CPQBOOKINGLINES</t>
+  </si>
+  <si>
+    <t>(5)</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -477,14 +483,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,6 +519,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -513,30 +595,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -553,64 +611,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -621,25 +627,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,25 +771,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,25 +783,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,91 +801,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,11 +834,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,6 +884,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,68 +931,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -946,128 +952,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1081,10 +1087,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
@@ -2243,13 +2249,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="26.6605504587156" customWidth="1"/>
     <col min="2" max="2" width="34.5045871559633" customWidth="1"/>
@@ -2312,13 +2318,24 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated CPQ test for QA env
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -423,10 +423,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -490,7 +490,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,22 +542,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,7 +565,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,54 +603,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -610,13 +617,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -627,6 +627,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -639,175 +801,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,41 +834,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -888,13 +858,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -904,6 +878,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,6 +914,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -934,7 +934,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -943,137 +946,134 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2252,7 +2252,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -2300,7 +2300,7 @@
         <v>126</v>
       </c>
       <c r="B4" s="2">
-        <v>2381626</v>
+        <v>2320020</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updated CPQ edited offering ID for QA; upgraded chromedriver.exe
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -423,10 +423,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -490,21 +490,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,6 +519,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -526,6 +535,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -542,14 +567,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -564,24 +582,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,29 +617,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -627,55 +627,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,42 +795,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -736,78 +808,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,6 +831,30 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -858,6 +882,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -869,15 +913,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -896,184 +931,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2252,7 +2252,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -2300,7 +2300,7 @@
         <v>126</v>
       </c>
       <c r="B4" s="2">
-        <v>2320020</v>
+        <v>2381626</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updated Reporter, added new PDF files added right mouse click action in SeleniumHelper
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="3"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
   <si>
     <t>Tag</t>
   </si>
@@ -238,6 +238,18 @@
     <t>12space34</t>
   </si>
   <si>
+    <t>QUARKUSER</t>
+  </si>
+  <si>
+    <t>yzosin</t>
+  </si>
+  <si>
+    <t>QUARKPASSWORD</t>
+  </si>
+  <si>
+    <t>Welcome8@</t>
+  </si>
+  <si>
     <t>ENTER</t>
   </si>
   <si>
@@ -383,6 +395,12 @@
   </si>
   <si>
     <t>https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view</t>
+  </si>
+  <si>
+    <t>QUARKURL</t>
+  </si>
+  <si>
+    <t>http://twaxqkpp401/workspace/login.qsp#</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -423,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -496,8 +514,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,14 +540,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -527,9 +554,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,15 +593,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,6 +601,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,57 +621,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -627,187 +645,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,11 +852,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -861,43 +918,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -917,24 +939,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -943,141 +967,135 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1093,24 +1111,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1122,12 +1146,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1432,10 +1456,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6605504587156" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1637,7 +1661,7 @@
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1659,7 +1683,7 @@
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1681,7 +1705,7 @@
       <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1791,7 +1815,7 @@
       <c r="A32" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -1813,7 +1837,7 @@
       <c r="A34" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -1835,7 +1859,7 @@
       <c r="A36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="18" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -1850,6 +1874,28 @@
         <v>72</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1897,10 +1943,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1908,10 +1954,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1919,10 +1965,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1930,10 +1976,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1941,10 +1987,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1952,10 +1998,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1963,10 +2009,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1982,10 +2028,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2008,10 +2054,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2019,10 +2065,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2030,10 +2076,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -2041,10 +2087,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2052,10 +2098,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2063,10 +2109,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2074,10 +2120,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2085,10 +2131,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2096,10 +2142,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2107,10 +2153,10 @@
     </row>
     <row r="11" s="6" customFormat="1" spans="1:3">
       <c r="A11" s="9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>5</v>
@@ -2118,10 +2164,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>5</v>
@@ -2129,10 +2175,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>5</v>
@@ -2140,10 +2186,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>5</v>
@@ -2151,10 +2197,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -2162,10 +2208,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>5</v>
@@ -2173,10 +2219,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="12" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>5</v>
@@ -2184,10 +2230,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -2195,10 +2241,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>5</v>
@@ -2206,10 +2252,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>5</v>
@@ -2217,12 +2263,23 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2239,6 +2296,7 @@
     <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
     <hyperlink ref="B20" r:id="rId9" display="http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/"/>
     <hyperlink ref="B21" r:id="rId10" display="https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view"/>
+    <hyperlink ref="B22" r:id="rId11" display="http://twaxqkpp401/workspace/login.qsp#"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2251,7 +2309,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2275,10 +2333,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2286,10 +2344,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2297,7 +2355,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B4" s="2">
         <v>2381626</v>
@@ -2308,10 +2366,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2319,10 +2377,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2330,10 +2388,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
created test for Quark added new Stepdefinitions
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
+    <workbookView windowWidth="20565" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
     <t>QUARKURL</t>
   </si>
   <si>
-    <t>http://twaxqkpp401/workspace/login.qsp#</t>
+    <t>7.0.12.124/workspace/login.qsp#</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -442,9 +442,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -500,20 +500,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -522,6 +508,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -530,22 +584,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -554,28 +592,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -585,29 +601,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,9 +615,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,6 +628,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -645,37 +645,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,139 +819,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,39 +868,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -918,8 +885,43 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -941,161 +943,159 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1127,12 +1127,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1462,12 +1456,12 @@
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6605504587156" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.65714285714286" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1651376146789" style="12" customWidth="1"/>
-    <col min="2" max="2" width="45.5045871559633" style="12" customWidth="1"/>
-    <col min="3" max="3" width="44.1651376146789" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="8.6605504587156" style="12"/>
+    <col min="1" max="1" width="38.1619047619048" style="12" customWidth="1"/>
+    <col min="2" max="2" width="45.5047619047619" style="12" customWidth="1"/>
+    <col min="3" max="3" width="44.1619047619048" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="8.65714285714286" style="12"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1661,7 +1655,7 @@
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1683,7 +1677,7 @@
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1705,7 +1699,7 @@
       <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1815,7 +1809,7 @@
       <c r="A32" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -1837,7 +1831,7 @@
       <c r="A34" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -1859,7 +1853,7 @@
       <c r="A36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -1923,10 +1917,10 @@
       <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.6605504587156" customWidth="1"/>
-    <col min="2" max="2" width="26.6605504587156" customWidth="1"/>
+    <col min="1" max="1" width="16.6571428571429" customWidth="1"/>
+    <col min="2" max="2" width="26.6571428571429" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1945,7 +1939,7 @@
       <c r="A2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2031,14 +2025,14 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="58.2752293577982" customWidth="1"/>
-    <col min="3" max="3" width="26.1651376146789" customWidth="1"/>
+    <col min="2" max="2" width="58.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="26.1619047619048" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2273,10 +2267,10 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -2296,7 +2290,7 @@
     <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
     <hyperlink ref="B20" r:id="rId9" display="http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/"/>
     <hyperlink ref="B21" r:id="rId10" display="https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view"/>
-    <hyperlink ref="B22" r:id="rId11" display="http://twaxqkpp401/workspace/login.qsp#"/>
+    <hyperlink ref="B22" r:id="rId11" display="7.0.12.124/workspace/login.qsp#"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2313,11 +2307,11 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="26.6605504587156" customWidth="1"/>
-    <col min="2" max="2" width="34.5045871559633" customWidth="1"/>
-    <col min="3" max="3" width="37.6605504587156" customWidth="1"/>
+    <col min="1" max="1" width="26.6571428571429" customWidth="1"/>
+    <col min="2" max="2" width="34.5047619047619" customWidth="1"/>
+    <col min="3" max="3" width="37.6571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
added new chromedriver; amended Qurk tests added new PDF base files
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20565" windowHeight="12330" activeTab="2"/>
+    <workbookView windowWidth="20565" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <t>QUARKPASSWORD</t>
   </si>
   <si>
-    <t>Welcome8@</t>
+    <t>Welcome9@</t>
   </si>
   <si>
     <t>ENTER</t>
@@ -441,8 +441,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -500,6 +500,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -508,15 +544,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,23 +622,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,81 +635,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -645,25 +645,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,49 +795,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,103 +825,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,41 +867,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -922,6 +887,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,149 +938,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1452,8 +1452,8 @@
   <sheetPr/>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65714285714286" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -2024,7 +2024,7 @@
   <sheetPr/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added CIMA files updated QUARK credentials
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20565" windowHeight="12330"/>
+    <workbookView windowWidth="21045" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <t>QUARKPASSWORD</t>
   </si>
   <si>
-    <t>Welcome9@</t>
+    <t>Welcome10@</t>
   </si>
   <si>
     <t>ENTER</t>
@@ -441,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -500,29 +500,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -538,6 +540,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -553,6 +563,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -567,6 +584,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -583,14 +608,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -599,38 +616,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,6 +645,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -657,175 +819,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,6 +849,45 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -894,45 +933,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -952,146 +952,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1452,8 +1452,8 @@
   <sheetPr/>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65714285714286" defaultRowHeight="15" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
updated PDF files after transfering to a new Web Platform edited test for Quark comparison added new Stepdef
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -241,7 +241,7 @@
     <t>QUARKUSER</t>
   </si>
   <si>
-    <t>yzosin</t>
+    <t>yuriizosin@bpp.com</t>
   </si>
   <si>
     <t>QUARKPASSWORD</t>
@@ -400,7 +400,7 @@
     <t>QUARKURL</t>
   </si>
   <si>
-    <t>7.0.12.124/workspace/login.qsp#</t>
+    <t>https://bpp-qa.app.quark.com/workspace/login.qsp#</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -441,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -500,6 +500,89 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -508,6 +591,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -517,70 +622,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -591,50 +635,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -645,187 +645,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,45 +849,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -933,6 +894,45 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -952,146 +952,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65714285714286" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1875,7 +1875,7 @@
       <c r="A38" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="16" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -1901,6 +1901,7 @@
     <hyperlink ref="B22" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
     <hyperlink ref="B32" r:id="rId4" display="nadineanja@yahoo.com"/>
     <hyperlink ref="B36" r:id="rId5" display="oksanasysadmincpq@bpp.com.noahqa"/>
+    <hyperlink ref="B38" r:id="rId6" display="yuriizosin@bpp.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2025,7 +2026,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -2290,7 +2291,7 @@
     <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
     <hyperlink ref="B20" r:id="rId9" display="http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/"/>
     <hyperlink ref="B21" r:id="rId10" display="https://bpp-13fd3e55182--noahqa.lightning.force.com/lightning/r/Instance__c/a43g00000008940AAA/view"/>
-    <hyperlink ref="B22" r:id="rId11" display="7.0.12.124/workspace/login.qsp#"/>
+    <hyperlink ref="B22" r:id="rId11" display="https://bpp-qa.app.quark.com/workspace/login.qsp#" tooltip="https://bpp-qa.app.quark.com/workspace/login.qsp#"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>